<commit_message>
Update tabel data RTL
</commit_message>
<xml_diff>
--- a/Document/tabel data RTL.xlsx
+++ b/Document/tabel data RTL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\workstation2\Documents\Oregano 8051 - SC Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4061B357-D3F3-47DB-AABA-22E7D537A5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09126FE-DA73-480B-B4F7-056A610A3CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{CFF6E223-DD87-428C-9022-0386BCC07B96}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Alamat SHD mem" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="MMI" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="190">
   <si>
     <t>Coprocessor</t>
   </si>
@@ -312,19 +315,329 @@
   </si>
   <si>
     <t>Hex</t>
+  </si>
+  <si>
+    <t>Arah</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>AES Encrypt text</t>
+  </si>
+  <si>
+    <t>3DES Chiper text</t>
+  </si>
+  <si>
+    <t>AES Decrypt Plaintext</t>
+  </si>
+  <si>
+    <t>XOR results</t>
+  </si>
+  <si>
+    <t>Remainder</t>
+  </si>
+  <si>
+    <t>Quotient</t>
+  </si>
+  <si>
+    <t>Multiplier Result</t>
+  </si>
+  <si>
+    <t>Add/Sub Result</t>
+  </si>
+  <si>
+    <t>HASH Output</t>
+  </si>
+  <si>
+    <t>3Des</t>
+  </si>
+  <si>
+    <t>XOR A</t>
+  </si>
+  <si>
+    <t>XOR B</t>
+  </si>
+  <si>
+    <t>Dividend</t>
+  </si>
+  <si>
+    <t>Divisor</t>
+  </si>
+  <si>
+    <t>Mul A</t>
+  </si>
+  <si>
+    <t>Mul B</t>
+  </si>
+  <si>
+    <t>Add/Sub A</t>
+  </si>
+  <si>
+    <t>Add/Sub B</t>
+  </si>
+  <si>
+    <t>HASH Input</t>
+  </si>
+  <si>
+    <t>AES Plaintect</t>
+  </si>
+  <si>
+    <t>AES Key</t>
+  </si>
+  <si>
+    <t>BC3 Input text</t>
+  </si>
+  <si>
+    <t>BC3 Output text</t>
+  </si>
+  <si>
+    <t>BC3 key</t>
+  </si>
+  <si>
+    <t>SHA1 Data</t>
+  </si>
+  <si>
+    <t>SHA1 CV</t>
+  </si>
+  <si>
+    <t>SHA1 out</t>
+  </si>
+  <si>
+    <t>3Des key</t>
+  </si>
+  <si>
+    <t>SHA1 CV0</t>
+  </si>
+  <si>
+    <t>ROM</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>00_0000_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>Internal register</t>
+  </si>
+  <si>
+    <t>01_0000_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>11_1111_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>NVM</t>
+  </si>
+  <si>
+    <t>00_0101_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>0_0000_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>0_0101_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>0_1000_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>1_1111_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>1_1111_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>0_1000_0000_0001_1111</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>0_0110_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>0_0111_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>0_1000_0000_0010_0000</t>
+  </si>
+  <si>
+    <t>0_1111_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>1_0010_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>1_0000_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>1_0011_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>1_0111_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>Lower Address(word)</t>
+  </si>
+  <si>
+    <t>Upper address(word)</t>
+  </si>
+  <si>
+    <t>Depth(KWord)</t>
+  </si>
+  <si>
+    <t>24K</t>
+  </si>
+  <si>
+    <t>8K</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>Lower (bin)</t>
+  </si>
+  <si>
+    <t>Upper (bin)</t>
+  </si>
+  <si>
+    <t>24 K</t>
+  </si>
+  <si>
+    <t>00_0110_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>00_0111_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>8 K</t>
+  </si>
+  <si>
+    <t>01_0000_0000_0000_0111</t>
+  </si>
+  <si>
+    <t>8 word</t>
+  </si>
+  <si>
+    <t>01_0000_0000_0000_1000</t>
+  </si>
+  <si>
+    <t>01_1111_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>10_0000_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>10_0010_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>12 K</t>
+  </si>
+  <si>
+    <t>10_0011_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>10_1111_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>11_1110_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>11_0000_0000_0000_0000</t>
+  </si>
+  <si>
+    <t>11_1101_1111_1111_1111</t>
+  </si>
+  <si>
+    <t>Lower (hex SS:AAAA)</t>
+  </si>
+  <si>
+    <t>Upper (hex SS:AAAA)</t>
+  </si>
+  <si>
+    <t>00:0x0000</t>
+  </si>
+  <si>
+    <t>00:0x5FFF</t>
+  </si>
+  <si>
+    <t>00:0x6000</t>
+  </si>
+  <si>
+    <t>00:0x7FFF</t>
+  </si>
+  <si>
+    <t>01:0x10000</t>
+  </si>
+  <si>
+    <t>01:0x10007</t>
+  </si>
+  <si>
+    <t>01:0x10008</t>
+  </si>
+  <si>
+    <t>01:0x1FFFF</t>
+  </si>
+  <si>
+    <t>10:0x20000</t>
+  </si>
+  <si>
+    <t>10:0x22FFF</t>
+  </si>
+  <si>
+    <t>10:0x23000</t>
+  </si>
+  <si>
+    <t>10:0x2FFFF</t>
+  </si>
+  <si>
+    <t>11:0x30000</t>
+  </si>
+  <si>
+    <t>11:0x3DFFF</t>
+  </si>
+  <si>
+    <t>11:0x3E000</t>
+  </si>
+  <si>
+    <t>11:0x3FFFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -341,7 +654,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -416,25 +729,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -778,7 +1144,7 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="25.453125" customWidth="1"/>
     <col min="2" max="2" width="24.7265625" customWidth="1"/>
@@ -786,7 +1152,7 @@
     <col min="5" max="5" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -800,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -814,7 +1180,7 @@
         <v>4712</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -828,7 +1194,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -842,7 +1208,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
@@ -850,7 +1216,7 @@
         <v>4239</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
@@ -858,7 +1224,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
@@ -866,7 +1232,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5">
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
@@ -874,7 +1240,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5">
       <c r="D12" t="s">
         <v>14</v>
       </c>
@@ -882,7 +1248,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5">
       <c r="D14" t="s">
         <v>15</v>
       </c>
@@ -891,7 +1257,7 @@
         <v>12218</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5">
       <c r="D15" t="s">
         <v>11</v>
       </c>
@@ -906,607 +1272,871 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DB4627-4958-4EDA-98CF-7EEC235D4C2A}">
-  <dimension ref="A3:F27"/>
+  <dimension ref="A3:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="2" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="3" width="7.90625" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" customWidth="1"/>
+    <col min="5" max="5" width="9.36328125" customWidth="1"/>
+    <col min="6" max="6" width="8.26953125" customWidth="1"/>
+    <col min="7" max="7" width="5.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="2" t="s">
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="5" spans="1:7">
+      <c r="A5" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="4">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="str">
-        <f>DEC2HEX(B5)</f>
+      <c r="D5" s="4" t="str">
+        <f>DEC2HEX(C5)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="4">
         <v>8</v>
       </c>
-      <c r="E5" s="2">
-        <f t="shared" ref="E5:E27" si="0">(B5+D5-1)</f>
+      <c r="F5" s="4">
+        <f t="shared" ref="F5:F34" si="0">(C5+E5-1)</f>
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="str">
-        <f>DEC2HEX(E5)</f>
+      <c r="G5" s="4" t="str">
+        <f>DEC2HEX(F5)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2">
-        <f>(E5+1)</f>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="4">
+        <f>(F5+1)</f>
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="str">
-        <f t="shared" ref="C6:C27" si="1">DEC2HEX(B6)</f>
+      <c r="D6" s="4" t="str">
+        <f t="shared" ref="D6:D30" si="1">DEC2HEX(C6)</f>
         <v>8</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="4">
         <v>8</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="F6" s="2" t="str">
-        <f t="shared" ref="F6:F27" si="2">DEC2HEX(E6)</f>
+      <c r="G6" s="4" t="str">
+        <f t="shared" ref="G6:G34" si="2">DEC2HEX(F6)</f>
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2">
-        <f t="shared" ref="B7:B25" si="3">(E6+1)</f>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" ref="C7:C16" si="3">(F6+1)</f>
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="str">
+      <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D7" s="2">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F7" s="2" t="str">
+      <c r="G7" s="4" t="str">
         <f t="shared" si="2"/>
         <v>2F</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="8" spans="1:7">
+      <c r="A8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="4">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="C8" s="2" t="str">
+      <c r="D8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="4">
         <v>16</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="F8" s="2" t="str">
+      <c r="G8" s="4" t="str">
         <f t="shared" si="2"/>
         <v>3F</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="9" spans="1:7">
+      <c r="A9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="4">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="C9" s="2" t="str">
+      <c r="D9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="4">
         <v>64</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>127</v>
       </c>
-      <c r="F9" s="2" t="str">
+      <c r="G9" s="4" t="str">
         <f t="shared" si="2"/>
         <v>7F</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="4">
         <f t="shared" si="3"/>
         <v>128</v>
       </c>
-      <c r="C10" s="2" t="str">
+      <c r="D10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="D10" s="2">
-        <v>32</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="E10" s="4">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>159</v>
       </c>
-      <c r="F10" s="2" t="str">
+      <c r="G10" s="4" t="str">
         <f t="shared" si="2"/>
         <v>9F</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="11" spans="1:7">
+      <c r="A11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="4">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="C11" s="2" t="str">
+      <c r="D11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>A0</v>
       </c>
-      <c r="D11" s="2">
-        <v>32</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="E11" s="4">
+        <v>32</v>
+      </c>
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>191</v>
       </c>
-      <c r="F11" s="2" t="str">
+      <c r="G11" s="4" t="str">
         <f t="shared" si="2"/>
         <v>BF</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="12" spans="1:7">
+      <c r="A12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="4">
         <f t="shared" si="3"/>
         <v>192</v>
       </c>
-      <c r="C12" s="2" t="str">
+      <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>C0</v>
       </c>
-      <c r="D12" s="2">
-        <v>32</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="E12" s="4">
+        <v>32</v>
+      </c>
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>223</v>
       </c>
-      <c r="F12" s="2" t="str">
+      <c r="G12" s="4" t="str">
         <f t="shared" si="2"/>
         <v>DF</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="13" spans="1:7">
+      <c r="A13" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="4">
         <f t="shared" si="3"/>
         <v>224</v>
       </c>
-      <c r="C13" s="2" t="str">
+      <c r="D13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>E0</v>
       </c>
-      <c r="D13" s="2">
-        <v>32</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
+        <v>32</v>
+      </c>
+      <c r="F13" s="4">
         <f t="shared" si="0"/>
         <v>255</v>
       </c>
-      <c r="F13" s="2" t="str">
-        <f t="shared" si="2"/>
+      <c r="G13" s="4" t="str">
+        <f>DEC2HEX(F13)</f>
         <v>FF</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2">
+    <row r="14" spans="1:7">
+      <c r="A14" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="4">
         <f t="shared" si="3"/>
         <v>256</v>
       </c>
-      <c r="C14" s="2" t="str">
+      <c r="D14" s="4" t="str">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="D14" s="2">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="E14" s="4">
+        <v>32</v>
+      </c>
+      <c r="F14" s="4">
         <f t="shared" si="0"/>
         <v>287</v>
       </c>
-      <c r="F14" s="2" t="str">
+      <c r="G14" s="4" t="str">
         <f t="shared" si="2"/>
         <v>11F</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2">
+    <row r="15" spans="1:7">
+      <c r="A15" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="4">
         <f t="shared" si="3"/>
         <v>288</v>
       </c>
-      <c r="C15" s="2" t="str">
+      <c r="D15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="D15" s="2">
-        <v>32</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="E15" s="4">
+        <v>32</v>
+      </c>
+      <c r="F15" s="4">
         <f t="shared" si="0"/>
         <v>319</v>
       </c>
-      <c r="F15" s="2" t="str">
+      <c r="G15" s="4" t="str">
         <f t="shared" si="2"/>
         <v>13F</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="2">
+    <row r="16" spans="1:7">
+      <c r="A16" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="4">
         <f t="shared" si="3"/>
         <v>320</v>
       </c>
-      <c r="C16" s="2" t="str">
+      <c r="D16" s="4" t="str">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="D16" s="2">
-        <v>32</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
+        <v>32</v>
+      </c>
+      <c r="F16" s="4">
         <f t="shared" si="0"/>
         <v>351</v>
       </c>
-      <c r="F16" s="2" t="str">
+      <c r="G16" s="4" t="str">
         <f t="shared" si="2"/>
         <v>15F</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2">
-        <f t="shared" si="3"/>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="4">
+        <f>(F16+1)</f>
         <v>352</v>
       </c>
-      <c r="C17" s="2" t="str">
+      <c r="D17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="D17" s="2">
-        <v>32</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="E17" s="4">
+        <v>32</v>
+      </c>
+      <c r="F17" s="4">
         <f t="shared" si="0"/>
         <v>383</v>
       </c>
-      <c r="F17" s="2" t="str">
+      <c r="G17" s="4" t="str">
         <f t="shared" si="2"/>
         <v>17F</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2">
-        <f t="shared" si="3"/>
+    <row r="18" spans="1:7">
+      <c r="A18" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" ref="C18:C34" si="4">(F17+1)</f>
         <v>384</v>
       </c>
-      <c r="C18" s="2" t="str">
+      <c r="D18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="4">
         <v>8</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="4">
         <f t="shared" si="0"/>
         <v>391</v>
       </c>
-      <c r="F18" s="2" t="str">
+      <c r="G18" s="4" t="str">
         <f t="shared" si="2"/>
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="2">
-        <f t="shared" si="3"/>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="4"/>
         <v>392</v>
       </c>
-      <c r="C19" s="2" t="str">
+      <c r="D19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>188</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="4">
+        <v>7</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="0"/>
+        <v>398</v>
+      </c>
+      <c r="G19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>18E</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="4"/>
+        <v>399</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>18F</v>
+      </c>
+      <c r="E20" s="4">
+        <v>64</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="0"/>
+        <v>462</v>
+      </c>
+      <c r="G20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1CE</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="4"/>
+        <v>463</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1CF</v>
+      </c>
+      <c r="E21" s="4">
+        <v>20</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="0"/>
+        <v>482</v>
+      </c>
+      <c r="G21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1E2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="4"/>
+        <v>483</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1E3</v>
+      </c>
+      <c r="E22" s="4">
+        <v>8</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="0"/>
+        <v>490</v>
+      </c>
+      <c r="G22" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1EA</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" si="4"/>
+        <v>491</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1EB</v>
+      </c>
+      <c r="E23" s="4">
         <v>16</v>
       </c>
-      <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>407</v>
-      </c>
-      <c r="F19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="2">
-        <f>(E19+1)</f>
-        <v>408</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>198</v>
-      </c>
-      <c r="D20" s="2">
-        <v>32</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>439</v>
-      </c>
-      <c r="F20" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>1B7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2">
-        <f t="shared" si="3"/>
-        <v>440</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>1B8</v>
-      </c>
-      <c r="D21" s="2">
-        <v>32</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="0"/>
-        <v>471</v>
-      </c>
-      <c r="F21" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>1D7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2">
-        <f>(E21+1)</f>
-        <v>472</v>
-      </c>
-      <c r="C22" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>1D8</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="F23" s="4">
+        <f t="shared" si="0"/>
+        <v>506</v>
+      </c>
+      <c r="G23" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1FA</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="4"/>
+        <v>507</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1FB</v>
+      </c>
+      <c r="E24" s="4">
+        <v>32</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="0"/>
+        <v>538</v>
+      </c>
+      <c r="G24" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>21A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="4"/>
+        <v>539</v>
+      </c>
+      <c r="D25" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>21B</v>
+      </c>
+      <c r="E25" s="4">
+        <v>32</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="0"/>
+        <v>570</v>
+      </c>
+      <c r="G25" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>23A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="4"/>
+        <v>571</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>23B</v>
+      </c>
+      <c r="E26" s="4">
         <v>64</v>
       </c>
-      <c r="E22" s="2">
-        <f t="shared" si="0"/>
-        <v>535</v>
-      </c>
-      <c r="F22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>217</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="2">
-        <f t="shared" si="3"/>
-        <v>536</v>
-      </c>
-      <c r="C23" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>218</v>
-      </c>
-      <c r="D23" s="2">
-        <v>32</v>
-      </c>
-      <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>567</v>
-      </c>
-      <c r="F23" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>237</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="2">
-        <f t="shared" si="3"/>
-        <v>568</v>
-      </c>
-      <c r="C24" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>238</v>
-      </c>
-      <c r="D24" s="2">
-        <v>32</v>
-      </c>
-      <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>599</v>
-      </c>
-      <c r="F24" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="2">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-      <c r="C25" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>258</v>
-      </c>
-      <c r="D25" s="2">
-        <v>32</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>631</v>
-      </c>
-      <c r="F25" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>277</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" s="2">
-        <v>632</v>
-      </c>
-      <c r="C26" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>278</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="F26" s="4">
+        <f t="shared" si="0"/>
+        <v>634</v>
+      </c>
+      <c r="G26" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>27A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="4"/>
+        <v>635</v>
+      </c>
+      <c r="D27" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>27B</v>
+      </c>
+      <c r="E27" s="4">
+        <v>32</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="0"/>
+        <v>666</v>
+      </c>
+      <c r="G27" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>29A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="4"/>
+        <v>667</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>29B</v>
+      </c>
+      <c r="E28" s="4">
+        <v>32</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="0"/>
+        <v>698</v>
+      </c>
+      <c r="G28" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>2BA</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="4"/>
+        <v>699</v>
+      </c>
+      <c r="D29" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>2BB</v>
+      </c>
+      <c r="E29" s="4">
+        <v>32</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="0"/>
+        <v>730</v>
+      </c>
+      <c r="G29" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>2DA</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="4"/>
+        <v>731</v>
+      </c>
+      <c r="D30" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>2DB</v>
+      </c>
+      <c r="E30" s="4">
         <v>4</v>
       </c>
-      <c r="E26" s="2">
-        <f t="shared" si="0"/>
-        <v>635</v>
-      </c>
-      <c r="F26" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>27B</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="2">
-        <v>636</v>
-      </c>
-      <c r="C27" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>27C</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="F30" s="4">
+        <f t="shared" si="0"/>
+        <v>734</v>
+      </c>
+      <c r="G30" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>2DE</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="4"/>
+        <v>735</v>
+      </c>
+      <c r="D31" s="4" t="str">
+        <f>DEC2HEX(C31)</f>
+        <v>2DF</v>
+      </c>
+      <c r="E31" s="4">
         <v>16</v>
       </c>
-      <c r="E27" s="2">
-        <f t="shared" si="0"/>
-        <v>651</v>
-      </c>
-      <c r="F27" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>28B</v>
+      <c r="F31" s="4">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="G31" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>2EE</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="4"/>
+        <v>751</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <f>DEC2HEX(C32)</f>
+        <v>2EF</v>
+      </c>
+      <c r="E32" s="4">
+        <v>8</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="0"/>
+        <v>758</v>
+      </c>
+      <c r="G32" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>2F6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="4"/>
+        <v>759</v>
+      </c>
+      <c r="D33" s="4" t="str">
+        <f>DEC2HEX(C33)</f>
+        <v>2F7</v>
+      </c>
+      <c r="E33" s="4">
+        <v>20</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="0"/>
+        <v>778</v>
+      </c>
+      <c r="G33" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>30A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="4"/>
+        <v>779</v>
+      </c>
+      <c r="D34" s="4" t="str">
+        <f>DEC2HEX(C34)</f>
+        <v>30B</v>
+      </c>
+      <c r="E34" s="7">
+        <v>20</v>
+      </c>
+      <c r="F34" s="4">
+        <f t="shared" si="0"/>
+        <v>798</v>
+      </c>
+      <c r="G34" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>31E</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
+  <mergeCells count="5">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1516,11 +2146,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4737F3-5D61-4CFB-B9DB-CB1DEACC34DE}">
   <dimension ref="A3:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14.36328125" customWidth="1"/>
     <col min="2" max="2" width="15.6328125" customWidth="1"/>
@@ -1528,7 +2158,7 @@
     <col min="4" max="4" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1542,7 +2172,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1557,7 +2187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1573,7 +2203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1589,7 +2219,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1605,7 +2235,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1621,7 +2251,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1637,7 +2267,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1653,7 +2283,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1669,7 +2299,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1685,7 +2315,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1701,7 +2331,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1717,7 +2347,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -1733,7 +2363,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1749,7 +2379,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1765,7 +2395,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>87</v>
       </c>
@@ -1781,7 +2411,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1797,7 +2427,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1813,7 +2443,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -1829,7 +2459,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
@@ -1845,7 +2475,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -1861,7 +2491,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1877,7 +2507,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>84</v>
       </c>
@@ -1893,7 +2523,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>88</v>
       </c>
@@ -1922,13 +2552,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.54296875" customWidth="1"/>
     <col min="2" max="4" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1942,7 +2572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1956,7 +2586,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1970,7 +2600,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1984,7 +2614,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1998,7 +2628,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2012,7 +2642,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2026,7 +2656,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2040,7 +2670,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2054,7 +2684,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2068,7 +2698,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2082,7 +2712,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2096,7 +2726,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2110,7 +2740,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2124,7 +2754,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2138,7 +2768,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2152,7 +2782,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2166,7 +2796,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2180,7 +2810,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -2194,7 +2824,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2208,7 +2838,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2222,7 +2852,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2236,7 +2866,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2248,6 +2878,481 @@
       </c>
       <c r="D23" t="s">
         <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA51DEE-DCF9-4653-8324-2539F4A9A027}">
+  <dimension ref="A2:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43473A51-7731-4D7B-83FA-9C7ED086FFDA}">
+  <dimension ref="A2:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.36328125" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175F4EE9-BFDD-441E-97D1-951C4F9DC383}">
+  <dimension ref="A2:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="29">
+      <c r="A2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>